<commit_message>
Adding missing component to buoy bom
</commit_message>
<xml_diff>
--- a/data-buoy-node/bill_of_materials.xlsx
+++ b/data-buoy-node/bill_of_materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdmed\Downloads\Uniandes\AsistenciaInvestigacion\OpenSourceDataBuoy\open-source-fish-farming-prototypes\data-buoy-node\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F65E8C5-CD64-4403-ACEE-10C517968230}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8251D43-964C-4961-8D42-5BB8147C27AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21600" xr2:uid="{CBC51B39-64A4-4F9B-B35D-416E43FC5AB9}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>Description</t>
   </si>
@@ -106,12 +106,6 @@
     <t>10L Polystyrene box</t>
   </si>
   <si>
-    <t>PVC Pipe 1 1/2" cut to 600mm length</t>
-  </si>
-  <si>
-    <t>PVC Pipe 1 1/2" cut to 180mm length</t>
-  </si>
-  <si>
     <t>PVC Male adapter 1 1/2"</t>
   </si>
   <si>
@@ -128,6 +122,18 @@
   </si>
   <si>
     <t>Cable Gland PG13.5</t>
+  </si>
+  <si>
+    <t>PVC cap 1 1/2"</t>
+  </si>
+  <si>
+    <t>PVC Pipe 3/4"</t>
+  </si>
+  <si>
+    <t>PVC Pipe 1 1/2"</t>
+  </si>
+  <si>
+    <t>1m</t>
   </si>
 </sst>
 </file>
@@ -241,10 +247,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -563,7 +569,7 @@
   <dimension ref="B2:D35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -574,10 +580,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="21" x14ac:dyDescent="0.5">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="8"/>
+      <c r="C2" s="9"/>
       <c r="D2" s="2"/>
     </row>
     <row r="4" spans="2:4" ht="18.5" x14ac:dyDescent="0.35">
@@ -615,7 +621,7 @@
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="1">
@@ -623,7 +629,7 @@
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="1">
@@ -639,7 +645,7 @@
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="1">
@@ -749,23 +755,23 @@
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="1">
-        <v>1</v>
+        <v>31</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" s="1">
-        <v>1</v>
+        <v>30</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C29" s="1">
         <v>1</v>
@@ -773,7 +779,7 @@
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C30" s="1">
         <v>2</v>
@@ -781,7 +787,7 @@
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C31" s="1">
         <v>2</v>
@@ -789,18 +795,23 @@
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C32" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C33" s="1"/>
+      <c r="B33" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C34" s="1">
         <v>1</v>
@@ -808,7 +819,7 @@
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C35" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
Adding Bill of Materials for Colombia.
</commit_message>
<xml_diff>
--- a/data-buoy-node/bill_of_materials.xlsx
+++ b/data-buoy-node/bill_of_materials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdmed\Downloads\Uniandes\AsistenciaInvestigacion\OpenSourceDataBuoy\open-source-fish-farming-prototypes\data-buoy-node\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8251D43-964C-4961-8D42-5BB8147C27AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4F2B50-AFE6-4D65-95E4-5BDB11407C60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21600" xr2:uid="{CBC51B39-64A4-4F9B-B35D-416E43FC5AB9}"/>
+    <workbookView xWindow="760" yWindow="0" windowWidth="19200" windowHeight="21600" xr2:uid="{CBC51B39-64A4-4F9B-B35D-416E43FC5AB9}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Description</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t>1m</t>
+  </si>
+  <si>
+    <t>RF cable SMA Male to SMA Female 15cm</t>
   </si>
 </sst>
 </file>
@@ -566,15 +569,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{753CFBDF-9549-4D5C-9A5F-E33649E0A1D6}">
-  <dimension ref="B2:D35"/>
+  <dimension ref="B2:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="32.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.90625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.26953125" customWidth="1"/>
   </cols>
@@ -614,47 +617,47 @@
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B9" s="8" t="s">
-        <v>14</v>
-      </c>
       <c r="C9" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B10" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B11" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B11" s="4" t="s">
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B12" s="8" t="s">
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B13" s="8" t="s">
         <v>20</v>
-      </c>
-      <c r="C12" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B13" s="4" t="s">
-        <v>19</v>
       </c>
       <c r="C13" s="1">
         <v>1</v>
@@ -662,7 +665,7 @@
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B14" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C14" s="1">
         <v>1</v>
@@ -670,55 +673,55 @@
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B16" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
-      <c r="B16" t="s">
-        <v>5</v>
-      </c>
       <c r="C16" s="1">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="1">
         <v>12</v>
       </c>
-      <c r="C17" s="1">
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="1">
         <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B18" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="1">
-        <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B19" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B20" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B20" t="s">
-        <v>8</v>
-      </c>
       <c r="C20" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C21" s="1">
         <v>2</v>
@@ -726,44 +729,44 @@
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C22" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C23" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="B25" s="5" t="s">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B26" s="5" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B26" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" s="1">
-        <v>1</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
-        <v>31</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>32</v>
+        <v>22</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>32</v>
@@ -771,23 +774,23 @@
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
-        <v>25</v>
-      </c>
-      <c r="C29" s="1">
-        <v>1</v>
+        <v>30</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C30" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C31" s="1">
         <v>2</v>
@@ -795,15 +798,15 @@
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C32" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C33" s="1">
         <v>1</v>
@@ -811,7 +814,7 @@
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C34" s="1">
         <v>1</v>
@@ -819,9 +822,17 @@
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
         <v>27</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C36" s="1">
         <v>1</v>
       </c>
     </row>
@@ -830,16 +841,17 @@
     <mergeCell ref="B2:C2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1" xr:uid="{EB3F6A4D-97AA-44BE-A763-0609BE91E514}"/>
-    <hyperlink ref="B19" r:id="rId2" xr:uid="{A5B1D517-FDBB-4C8C-BE25-ECED92961C20}"/>
+    <hyperlink ref="B9" r:id="rId1" xr:uid="{EB3F6A4D-97AA-44BE-A763-0609BE91E514}"/>
+    <hyperlink ref="B20" r:id="rId2" xr:uid="{A5B1D517-FDBB-4C8C-BE25-ECED92961C20}"/>
     <hyperlink ref="B7" r:id="rId3" xr:uid="{0CEABB27-7CFF-4581-8AAF-FD5F08FBFEEF}"/>
-    <hyperlink ref="B18" r:id="rId4" xr:uid="{F7984E46-E949-4707-AB1E-74EA84C0708E}"/>
-    <hyperlink ref="B11" r:id="rId5" xr:uid="{63B03883-CBBF-4CE6-81EA-37D233FC4123}"/>
-    <hyperlink ref="B14" r:id="rId6" xr:uid="{3232244A-B12C-4414-B96C-B7C82C176471}"/>
-    <hyperlink ref="B15" r:id="rId7" xr:uid="{D8876DD3-ECDB-4B75-A07C-4D1FA3E11B62}"/>
-    <hyperlink ref="B13" r:id="rId8" xr:uid="{512A2924-0EC8-43CF-81AA-D4DBEA3DB861}"/>
+    <hyperlink ref="B19" r:id="rId4" xr:uid="{F7984E46-E949-4707-AB1E-74EA84C0708E}"/>
+    <hyperlink ref="B12" r:id="rId5" xr:uid="{63B03883-CBBF-4CE6-81EA-37D233FC4123}"/>
+    <hyperlink ref="B15" r:id="rId6" xr:uid="{3232244A-B12C-4414-B96C-B7C82C176471}"/>
+    <hyperlink ref="B16" r:id="rId7" xr:uid="{D8876DD3-ECDB-4B75-A07C-4D1FA3E11B62}"/>
+    <hyperlink ref="B14" r:id="rId8" xr:uid="{512A2924-0EC8-43CF-81AA-D4DBEA3DB861}"/>
+    <hyperlink ref="B8" r:id="rId9" xr:uid="{B2507739-0A55-4468-B832-FF854CBF6D68}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId9"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>